<commit_message>
Actualizacion encuesta de satisfaccion por error en nombre de entrevistado
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Encuestas de Satisfaccion/Cinovatec_EncuestaSatisfaccion-150624.xlsx
+++ b/qualtcom/Procesos/Encuestas de Satisfaccion/Cinovatec_EncuestaSatisfaccion-150624.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="817" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="817" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Inf. Gral." sheetId="1" r:id="rId1"/>
@@ -232,9 +232,6 @@
     <t>Describir aquí las cosas que el cliente comenta acerca de la pregunta que se acaba de realizar. Escribir textualmente los comentarios del entrevistado buscando quedar claro en lo que desea expresar</t>
   </si>
   <si>
-    <t>Mariano Soto</t>
-  </si>
-  <si>
     <t>Mayra Tejeda</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Adriana Lira Beltran</t>
   </si>
 </sst>
 </file>
@@ -1495,7 +1495,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="125" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="125"/>
       <c r="E5" s="125"/>
@@ -1506,13 +1506,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="125" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="125"/>
       <c r="E6" s="125"/>
       <c r="F6" s="125"/>
       <c r="G6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1531,7 +1531,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="125" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" s="125"/>
       <c r="E8" s="125"/>
@@ -1679,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1795,7 +1795,7 @@
       <c r="A4" s="103"/>
       <c r="B4" s="103"/>
       <c r="C4" s="92" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -1870,7 +1870,7 @@
       <c r="A5" s="104"/>
       <c r="B5" s="104"/>
       <c r="C5" s="93" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -10300,7 +10300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>